<commit_message>
lareptm con la Apa
</commit_message>
<xml_diff>
--- a/assets uarm/filrel2018b controles.xlsx
+++ b/assets uarm/filrel2018b controles.xlsx
@@ -503,7 +503,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -529,15 +529,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -552,6 +543,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -849,7 +852,7 @@
   <dimension ref="A1:AD20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X23" sqref="X23"/>
+      <selection activeCell="G12" sqref="G12:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -881,41 +884,41 @@
       <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="25" t="s">
+      <c r="E2" s="40"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="25" t="s">
+      <c r="H2" s="40"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="26"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="25" t="s">
+      <c r="K2" s="40"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="26"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="25" t="s">
+      <c r="N2" s="40"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="25" t="s">
+      <c r="Q2" s="40"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="26"/>
-      <c r="U2" s="27"/>
-      <c r="V2" s="25" t="s">
+      <c r="T2" s="40"/>
+      <c r="U2" s="41"/>
+      <c r="V2" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="W2" s="26"/>
-      <c r="X2" s="27"/>
+      <c r="W2" s="40"/>
+      <c r="X2" s="41"/>
       <c r="Y2" s="7" t="s">
         <v>31</v>
       </c>
@@ -925,10 +928,10 @@
       <c r="AA2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AB2" s="39" t="s">
+      <c r="AB2" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="AC2" s="39" t="s">
+      <c r="AC2" s="36" t="s">
         <v>35</v>
       </c>
       <c r="AD2" s="3" t="s">
@@ -1079,7 +1082,7 @@
         <v>1.5</v>
       </c>
       <c r="Y4" s="14">
-        <f>SUM(D4:X4)</f>
+        <f t="shared" ref="Y4:Y20" si="0">SUM(D4:X4)</f>
         <v>17.5</v>
       </c>
       <c r="Z4" s="12">
@@ -1093,29 +1096,29 @@
       </c>
     </row>
     <row r="5" spans="1:30">
-      <c r="A5" s="35">
+      <c r="A5" s="32">
         <v>1</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36" t="s">
+      <c r="B5" s="33"/>
+      <c r="C5" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="E5" s="35">
-        <v>0.5</v>
-      </c>
-      <c r="F5" s="38">
-        <v>1.5</v>
-      </c>
-      <c r="G5" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="H5" s="35">
-        <v>0.5</v>
-      </c>
-      <c r="I5" s="38">
+      <c r="D5" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="35">
+        <v>1.5</v>
+      </c>
+      <c r="G5" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="H5" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="I5" s="35">
         <v>1.3</v>
       </c>
       <c r="J5" s="21">
@@ -1124,58 +1127,58 @@
       <c r="K5" s="21">
         <v>0.5</v>
       </c>
-      <c r="L5" s="38">
+      <c r="L5" s="35">
         <v>1.2</v>
       </c>
-      <c r="M5" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="N5" s="35">
-        <v>0</v>
-      </c>
-      <c r="O5" s="38">
-        <v>1.5</v>
-      </c>
-      <c r="P5" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="Q5" s="35">
-        <v>0</v>
-      </c>
-      <c r="R5" s="38">
+      <c r="M5" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="N5" s="32">
+        <v>0</v>
+      </c>
+      <c r="O5" s="35">
+        <v>1.5</v>
+      </c>
+      <c r="P5" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="Q5" s="32">
+        <v>0</v>
+      </c>
+      <c r="R5" s="35">
         <v>1.4</v>
       </c>
-      <c r="S5" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="T5" s="35">
-        <v>0</v>
-      </c>
-      <c r="U5" s="38">
+      <c r="S5" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="T5" s="32">
+        <v>0</v>
+      </c>
+      <c r="U5" s="35">
         <v>1.4</v>
       </c>
-      <c r="V5" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="W5" s="35">
-        <v>0.5</v>
-      </c>
-      <c r="X5" s="38">
+      <c r="V5" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="W5" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="X5" s="35">
         <v>1.2</v>
       </c>
       <c r="Y5" s="9">
-        <f>SUM(D5:X5)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="Z5" s="8">
         <v>2</v>
       </c>
       <c r="AA5" s="8">
-        <f>SUM(Y5:Z5)</f>
+        <f t="shared" ref="AA5:AA20" si="1">SUM(Y5:Z5)</f>
         <v>17</v>
       </c>
-      <c r="AB5" s="40"/>
-      <c r="AD5" s="36" t="s">
+      <c r="AB5" s="37"/>
+      <c r="AD5" s="33" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1187,45 +1190,51 @@
       <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="E6" s="29">
-        <v>0.5</v>
-      </c>
-      <c r="F6" s="30">
+      <c r="D6" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="27">
         <v>1.4</v>
       </c>
-      <c r="G6" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="H6" s="29">
-        <v>0.5</v>
-      </c>
-      <c r="I6" s="30">
-        <v>1.5</v>
-      </c>
-      <c r="J6" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="K6" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="L6" s="30">
+      <c r="G6" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="H6" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="I6" s="27">
+        <v>1.5</v>
+      </c>
+      <c r="J6" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="K6" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="L6" s="27">
         <v>1.3</v>
       </c>
-      <c r="M6" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="N6" s="29">
-        <v>0</v>
-      </c>
-      <c r="O6" s="30">
-        <v>1.5</v>
-      </c>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="17"/>
+      <c r="M6" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="N6" s="26">
+        <v>0</v>
+      </c>
+      <c r="O6" s="27">
+        <v>1.5</v>
+      </c>
+      <c r="P6" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="Q6" s="43">
+        <v>0</v>
+      </c>
+      <c r="R6" s="44">
+        <v>1</v>
+      </c>
       <c r="S6" s="15"/>
       <c r="T6" s="16"/>
       <c r="U6" s="17"/>
@@ -1233,15 +1242,15 @@
       <c r="W6" s="16"/>
       <c r="X6" s="17"/>
       <c r="Y6" s="4">
-        <f>SUM(D6:X6)</f>
-        <v>9.1999999999999993</v>
+        <f t="shared" si="0"/>
+        <v>10.7</v>
       </c>
       <c r="Z6" s="8">
         <v>2</v>
       </c>
       <c r="AA6" s="1">
-        <f>SUM(Y6:Z6)</f>
-        <v>11.2</v>
+        <f t="shared" si="1"/>
+        <v>12.7</v>
       </c>
       <c r="AD6" s="3" t="s">
         <v>7</v>
@@ -1251,8 +1260,8 @@
       <c r="A7" s="22">
         <v>3</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34" t="s">
+      <c r="B7" s="31"/>
+      <c r="C7" s="31" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="21">
@@ -1319,93 +1328,105 @@
         <v>1.4</v>
       </c>
       <c r="Y7" s="4">
-        <f>SUM(D7:X7)</f>
+        <f t="shared" si="0"/>
         <v>14.900000000000002</v>
       </c>
       <c r="Z7" s="8">
         <v>2.5</v>
       </c>
       <c r="AA7" s="1">
-        <f>SUM(Y7:Z7)</f>
+        <f t="shared" si="1"/>
         <v>17.400000000000002</v>
       </c>
-      <c r="AB7" s="40"/>
-      <c r="AD7" s="34" t="s">
+      <c r="AB7" s="37"/>
+      <c r="AD7" s="31" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:30">
-      <c r="A8" s="1">
+      <c r="A8" s="22">
         <v>4</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="31"/>
+      <c r="C8" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="E8" s="29">
-        <v>0.5</v>
-      </c>
-      <c r="F8" s="30">
-        <v>1.5</v>
-      </c>
-      <c r="G8" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="H8" s="29">
-        <v>0.5</v>
-      </c>
-      <c r="I8" s="30">
+      <c r="D8" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="23">
+        <v>1.5</v>
+      </c>
+      <c r="G8" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="H8" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="I8" s="23">
         <v>1.3</v>
       </c>
-      <c r="J8" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="K8" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="L8" s="30">
+      <c r="J8" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="K8" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="L8" s="23">
         <v>1.3</v>
       </c>
-      <c r="M8" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="N8" s="29">
-        <v>0</v>
-      </c>
-      <c r="O8" s="30">
+      <c r="M8" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="N8" s="22">
+        <v>0</v>
+      </c>
+      <c r="O8" s="23">
         <v>1.2</v>
       </c>
-      <c r="P8" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="Q8" s="29">
-        <v>0</v>
-      </c>
-      <c r="R8" s="30">
+      <c r="P8" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="Q8" s="22">
+        <v>0</v>
+      </c>
+      <c r="R8" s="23">
         <v>1.4</v>
       </c>
-      <c r="S8" s="15"/>
-      <c r="T8" s="16"/>
-      <c r="U8" s="17"/>
-      <c r="V8" s="15"/>
-      <c r="W8" s="16"/>
-      <c r="X8" s="17"/>
+      <c r="S8" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="T8" s="22">
+        <v>0</v>
+      </c>
+      <c r="U8" s="23">
+        <v>1.2</v>
+      </c>
+      <c r="V8" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="W8" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="X8" s="23">
+        <v>1.3</v>
+      </c>
       <c r="Y8" s="4">
-        <f>SUM(D8:X8)</f>
-        <v>10.7</v>
+        <f t="shared" si="0"/>
+        <v>14.7</v>
       </c>
       <c r="Z8" s="8">
         <v>2</v>
       </c>
       <c r="AA8" s="1">
-        <f>SUM(Y8:Z8)</f>
-        <v>12.7</v>
-      </c>
-      <c r="AB8" s="40"/>
-      <c r="AD8" s="3" t="s">
+        <f t="shared" si="1"/>
+        <v>16.7</v>
+      </c>
+      <c r="AB8" s="37"/>
+      <c r="AD8" s="31" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1413,8 +1434,8 @@
       <c r="A9" s="22">
         <v>5</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34" t="s">
+      <c r="B9" s="31"/>
+      <c r="C9" s="31" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="21">
@@ -1481,18 +1502,18 @@
         <v>1.4</v>
       </c>
       <c r="Y9" s="4">
-        <f>SUM(D9:X9)</f>
+        <f t="shared" si="0"/>
         <v>15.200000000000001</v>
       </c>
       <c r="Z9" s="8">
         <v>2.5</v>
       </c>
       <c r="AA9" s="1">
-        <f>SUM(Y9:Z9)</f>
+        <f t="shared" si="1"/>
         <v>17.700000000000003</v>
       </c>
-      <c r="AB9" s="40"/>
-      <c r="AD9" s="34" t="s">
+      <c r="AB9" s="37"/>
+      <c r="AD9" s="31" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1500,8 +1521,8 @@
       <c r="A10" s="22">
         <v>6</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34" t="s">
+      <c r="B10" s="31"/>
+      <c r="C10" s="31" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="21">
@@ -1568,18 +1589,18 @@
         <v>1.5</v>
       </c>
       <c r="Y10" s="4">
-        <f>SUM(D10:X10)</f>
+        <f t="shared" si="0"/>
         <v>14.2</v>
       </c>
       <c r="Z10" s="8">
         <v>2.5</v>
       </c>
       <c r="AA10" s="1">
-        <f>SUM(Y10:Z10)</f>
+        <f t="shared" si="1"/>
         <v>16.7</v>
       </c>
-      <c r="AB10" s="40"/>
-      <c r="AD10" s="34" t="s">
+      <c r="AB10" s="37"/>
+      <c r="AD10" s="31" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1591,69 +1612,81 @@
       <c r="C11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="E11" s="29">
-        <v>0.5</v>
-      </c>
-      <c r="F11" s="30">
+      <c r="D11" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="F11" s="23">
         <v>1.4</v>
       </c>
-      <c r="G11" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="H11" s="29">
-        <v>0</v>
-      </c>
-      <c r="I11" s="30">
+      <c r="G11" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="H11" s="22">
+        <v>0</v>
+      </c>
+      <c r="I11" s="23">
         <v>1.3</v>
       </c>
-      <c r="J11" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="K11" s="29">
-        <v>0.5</v>
-      </c>
-      <c r="L11" s="30">
+      <c r="J11" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="K11" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="L11" s="23">
         <v>1.2</v>
       </c>
-      <c r="M11" s="15"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="T11" s="29">
-        <v>0</v>
-      </c>
-      <c r="U11" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="V11" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="W11" s="29">
-        <v>0.5</v>
-      </c>
-      <c r="X11" s="30">
+      <c r="M11" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="N11" s="22">
+        <v>0</v>
+      </c>
+      <c r="O11" s="23">
+        <v>1.3</v>
+      </c>
+      <c r="P11" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="Q11" s="22">
+        <v>0</v>
+      </c>
+      <c r="R11" s="23">
+        <v>1.2</v>
+      </c>
+      <c r="S11" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="T11" s="22">
+        <v>0</v>
+      </c>
+      <c r="U11" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="V11" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="W11" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="X11" s="23">
         <v>1.5</v>
       </c>
       <c r="Y11" s="4">
-        <f>SUM(D11:X11)</f>
-        <v>9.9</v>
+        <f t="shared" si="0"/>
+        <v>13.4</v>
       </c>
       <c r="Z11" s="8">
         <v>1</v>
       </c>
       <c r="AA11" s="1">
-        <f>SUM(Y11:Z11)</f>
-        <v>10.9</v>
-      </c>
-      <c r="AB11" s="40"/>
+        <f t="shared" si="1"/>
+        <v>14.4</v>
+      </c>
+      <c r="AB11" s="37"/>
       <c r="AD11" s="3" t="s">
         <v>12</v>
       </c>
@@ -1666,28 +1699,34 @@
       <c r="C12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="E12" s="29">
-        <v>0.5</v>
-      </c>
-      <c r="F12" s="30">
+      <c r="D12" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="E12" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="F12" s="27">
         <v>1.4</v>
       </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="17"/>
+      <c r="G12" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="H12" s="43">
+        <v>0</v>
+      </c>
+      <c r="I12" s="44">
+        <v>1.4</v>
+      </c>
       <c r="J12" s="15"/>
       <c r="K12" s="16"/>
       <c r="L12" s="17"/>
-      <c r="M12" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="N12" s="29">
-        <v>0.5</v>
-      </c>
-      <c r="O12" s="30">
+      <c r="M12" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="N12" s="43">
+        <v>0.5</v>
+      </c>
+      <c r="O12" s="44">
         <v>1.3</v>
       </c>
       <c r="P12" s="15"/>
@@ -1700,17 +1739,17 @@
       <c r="W12" s="16"/>
       <c r="X12" s="17"/>
       <c r="Y12" s="4">
-        <f>SUM(D12:X12)</f>
-        <v>4.7</v>
+        <f t="shared" si="0"/>
+        <v>6.6</v>
       </c>
       <c r="Z12" s="8">
         <v>2.5</v>
       </c>
       <c r="AA12" s="1">
-        <f>SUM(Y12:Z12)</f>
-        <v>7.2</v>
-      </c>
-      <c r="AB12" s="40"/>
+        <f t="shared" si="1"/>
+        <v>9.1</v>
+      </c>
+      <c r="AB12" s="37"/>
       <c r="AD12" s="3" t="s">
         <v>13</v>
       </c>
@@ -1723,36 +1762,36 @@
       <c r="C13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="E13" s="29">
-        <v>0.5</v>
-      </c>
-      <c r="F13" s="30">
+      <c r="D13" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="F13" s="27">
         <v>1.4</v>
       </c>
-      <c r="G13" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="H13" s="29">
-        <v>0.5</v>
-      </c>
-      <c r="I13" s="30">
-        <v>1.5</v>
-      </c>
-      <c r="J13" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="K13" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="L13" s="30">
+      <c r="G13" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="H13" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="I13" s="27">
+        <v>1.5</v>
+      </c>
+      <c r="J13" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="K13" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="L13" s="27">
         <v>1.3</v>
       </c>
-      <c r="M13" s="41"/>
-      <c r="N13" s="41"/>
-      <c r="O13" s="41"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="38"/>
+      <c r="O13" s="38"/>
       <c r="P13" s="15"/>
       <c r="Q13" s="16"/>
       <c r="R13" s="17"/>
@@ -1763,17 +1802,17 @@
       <c r="W13" s="16"/>
       <c r="X13" s="17"/>
       <c r="Y13" s="4">
-        <f>SUM(D13:X13)</f>
+        <f t="shared" si="0"/>
         <v>7.2</v>
       </c>
       <c r="Z13" s="8">
         <v>2.5</v>
       </c>
       <c r="AA13" s="1">
-        <f>SUM(Y13:Z13)</f>
+        <f t="shared" si="1"/>
         <v>9.6999999999999993</v>
       </c>
-      <c r="AB13" s="40"/>
+      <c r="AB13" s="37"/>
       <c r="AD13" s="3" t="s">
         <v>14</v>
       </c>
@@ -1782,8 +1821,8 @@
       <c r="A14" s="22">
         <v>10</v>
       </c>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34" t="s">
+      <c r="B14" s="31"/>
+      <c r="C14" s="31" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="21">
@@ -1850,18 +1889,18 @@
         <v>1.5</v>
       </c>
       <c r="Y14" s="4">
-        <f>SUM(D14:X14)</f>
+        <f t="shared" si="0"/>
         <v>14.100000000000001</v>
       </c>
       <c r="Z14" s="8">
         <v>1</v>
       </c>
       <c r="AA14" s="1">
-        <f>SUM(Y14:Z14)</f>
+        <f t="shared" si="1"/>
         <v>15.100000000000001</v>
       </c>
-      <c r="AB14" s="40"/>
-      <c r="AD14" s="34" t="s">
+      <c r="AB14" s="37"/>
+      <c r="AD14" s="31" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1873,27 +1912,27 @@
       <c r="C15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="E15" s="29">
-        <v>0.5</v>
-      </c>
-      <c r="F15" s="30">
+      <c r="D15" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="E15" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="27">
         <v>1.3</v>
       </c>
-      <c r="G15" s="28"/>
-      <c r="H15" s="29">
-        <v>0</v>
-      </c>
-      <c r="I15" s="30"/>
-      <c r="J15" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="K15" s="28">
-        <v>0</v>
-      </c>
-      <c r="L15" s="30">
+      <c r="G15" s="25"/>
+      <c r="H15" s="26">
+        <v>0</v>
+      </c>
+      <c r="I15" s="27"/>
+      <c r="J15" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="K15" s="25">
+        <v>0</v>
+      </c>
+      <c r="L15" s="27">
         <v>0.9</v>
       </c>
       <c r="M15" s="15"/>
@@ -1909,17 +1948,17 @@
       <c r="W15" s="16"/>
       <c r="X15" s="17"/>
       <c r="Y15" s="4">
-        <f>SUM(D15:X15)</f>
+        <f t="shared" si="0"/>
         <v>3.6999999999999997</v>
       </c>
       <c r="Z15" s="8">
         <v>1</v>
       </c>
       <c r="AA15" s="1">
-        <f>SUM(Y15:Z15)</f>
+        <f t="shared" si="1"/>
         <v>4.6999999999999993</v>
       </c>
-      <c r="AB15" s="40"/>
+      <c r="AB15" s="37"/>
       <c r="AD15" s="3" t="s">
         <v>16</v>
       </c>
@@ -1932,31 +1971,31 @@
       <c r="C16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="E16" s="29">
-        <v>0.5</v>
-      </c>
-      <c r="F16" s="30">
-        <v>1.5</v>
-      </c>
-      <c r="G16" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="H16" s="29">
-        <v>0.5</v>
-      </c>
-      <c r="I16" s="30">
-        <v>1.5</v>
-      </c>
-      <c r="J16" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="K16" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="L16" s="30">
+      <c r="D16" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="E16" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="F16" s="27">
+        <v>1.5</v>
+      </c>
+      <c r="G16" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="H16" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="I16" s="27">
+        <v>1.5</v>
+      </c>
+      <c r="J16" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="K16" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="L16" s="27">
         <v>1.3</v>
       </c>
       <c r="M16" s="15"/>
@@ -1965,30 +2004,30 @@
       <c r="P16" s="15"/>
       <c r="Q16" s="16"/>
       <c r="R16" s="17"/>
-      <c r="S16" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="T16" s="29">
-        <v>0.5</v>
-      </c>
-      <c r="U16" s="30">
+      <c r="S16" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="T16" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="U16" s="27">
         <v>1.4</v>
       </c>
       <c r="V16" s="15"/>
       <c r="W16" s="16"/>
       <c r="X16" s="17"/>
       <c r="Y16" s="4">
-        <f>SUM(D16:X16)</f>
+        <f t="shared" si="0"/>
         <v>9.7000000000000011</v>
       </c>
       <c r="Z16" s="8">
         <v>2.5</v>
       </c>
       <c r="AA16" s="1">
-        <f>SUM(Y16:Z16)</f>
+        <f t="shared" si="1"/>
         <v>12.200000000000001</v>
       </c>
-      <c r="AB16" s="40"/>
+      <c r="AB16" s="37"/>
       <c r="AD16" s="3" t="s">
         <v>17</v>
       </c>
@@ -2029,17 +2068,17 @@
       <c r="W17" s="16"/>
       <c r="X17" s="17"/>
       <c r="Y17" s="4">
-        <f>SUM(D17:X17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Z17" s="8">
         <v>0</v>
       </c>
       <c r="AA17" s="1">
-        <f>SUM(Y17:Z17)</f>
-        <v>0</v>
-      </c>
-      <c r="AB17" s="40"/>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB17" s="37"/>
       <c r="AD17" s="3" t="s">
         <v>18</v>
       </c>
@@ -2048,8 +2087,8 @@
       <c r="A18" s="22">
         <v>14</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34" t="s">
+      <c r="B18" s="31"/>
+      <c r="C18" s="31" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="21">
@@ -2116,18 +2155,18 @@
         <v>1.2</v>
       </c>
       <c r="Y18" s="4">
-        <f>SUM(D18:X18)</f>
+        <f t="shared" si="0"/>
         <v>14.299999999999999</v>
       </c>
       <c r="Z18" s="8">
         <v>2.5</v>
       </c>
       <c r="AA18" s="1">
-        <f>SUM(Y18:Z18)</f>
+        <f t="shared" si="1"/>
         <v>16.799999999999997</v>
       </c>
-      <c r="AB18" s="40"/>
-      <c r="AD18" s="34" t="s">
+      <c r="AB18" s="37"/>
+      <c r="AD18" s="31" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2135,8 +2174,8 @@
       <c r="A19" s="22">
         <v>15</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34" t="s">
+      <c r="B19" s="31"/>
+      <c r="C19" s="31" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="21">
@@ -2203,18 +2242,18 @@
         <v>1.5</v>
       </c>
       <c r="Y19" s="4">
-        <f>SUM(D19:X19)</f>
+        <f t="shared" si="0"/>
         <v>15.4</v>
       </c>
       <c r="Z19" s="8">
         <v>2.5</v>
       </c>
       <c r="AA19" s="1">
-        <f>SUM(Y19:Z19)</f>
+        <f t="shared" si="1"/>
         <v>17.899999999999999</v>
       </c>
-      <c r="AB19" s="40"/>
-      <c r="AD19" s="34" t="s">
+      <c r="AB19" s="37"/>
+      <c r="AD19" s="31" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2226,22 +2265,22 @@
       <c r="C20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="31">
-        <v>0.5</v>
-      </c>
-      <c r="E20" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="F20" s="33">
-        <v>1.5</v>
-      </c>
-      <c r="G20" s="31">
-        <v>0.5</v>
-      </c>
-      <c r="H20" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="I20" s="33">
+      <c r="D20" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="E20" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="F20" s="30">
+        <v>1.5</v>
+      </c>
+      <c r="G20" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="H20" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="I20" s="30">
         <v>1.5</v>
       </c>
       <c r="J20" s="18"/>
@@ -2262,17 +2301,17 @@
       <c r="W20" s="19"/>
       <c r="X20" s="20"/>
       <c r="Y20" s="4">
-        <f>SUM(D20:X20)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="Z20" s="8">
         <v>2.5</v>
       </c>
       <c r="AA20" s="1">
-        <f>SUM(Y20:Z20)</f>
+        <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
-      <c r="AB20" s="40"/>
+      <c r="AB20" s="37"/>
       <c r="AD20" s="3" t="s">
         <v>21</v>
       </c>

</xml_diff>